<commit_message>
DEV-213 - import historical data from ftp
</commit_message>
<xml_diff>
--- a/src/exchange/tests/files/division.xlsx
+++ b/src/exchange/tests/files/division.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Лист1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Лист1!$A$1:$B$5</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Лист1!$A$1:$B$6</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">Код магазина</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t xml:space="preserve">07e6d8fc-87d9-11eb-80bb-0050568a6492</t>
+  </si>
+  <si>
+    <t xml:space="preserve">938e3dcd-6824-11ea-80e8-0050568ab54f</t>
   </si>
   <si>
     <t xml:space="preserve">Код, которого нету</t>
@@ -151,7 +154,7 @@
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -185,31 +188,38 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>194</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
         <v>539</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="ALU4" s="0"/>
-      <c r="ALV4" s="0"/>
-      <c r="ALW4" s="0"/>
-      <c r="ALX4" s="0"/>
-      <c r="ALY4" s="0"/>
-      <c r="ALZ4" s="0"/>
-      <c r="AMA4" s="0"/>
-      <c r="AMB4" s="0"/>
-      <c r="AMC4" s="0"/>
-      <c r="AMD4" s="0"/>
-      <c r="AME4" s="0"/>
-      <c r="AMF4" s="0"/>
-      <c r="AMG4" s="0"/>
-      <c r="AMH4" s="0"/>
-      <c r="AMI4" s="0"/>
-      <c r="AMJ4" s="0"/>
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="ALU5" s="0"/>
+      <c r="ALV5" s="0"/>
+      <c r="ALW5" s="0"/>
+      <c r="ALX5" s="0"/>
+      <c r="ALY5" s="0"/>
+      <c r="ALZ5" s="0"/>
+      <c r="AMA5" s="0"/>
+      <c r="AMB5" s="0"/>
+      <c r="AMC5" s="0"/>
+      <c r="AMD5" s="0"/>
+      <c r="AME5" s="0"/>
+      <c r="AMF5" s="0"/>
+      <c r="AMG5" s="0"/>
+      <c r="AMH5" s="0"/>
+      <c r="AMI5" s="0"/>
+      <c r="AMJ5" s="0"/>
     </row>
-    <row r="1048310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -477,7 +487,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:B5"/>
+  <autoFilter ref="A1:B6"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>